<commit_message>
add SEL keywords, clarify ongoing/completed in template
</commit_message>
<xml_diff>
--- a/standards/keyword_thesauri.xlsx
+++ b/standards/keyword_thesauri.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmaurer/GitHub/jrn_metadata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmaurer/GitHub/documentation/standards/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20D41427-14E1-E34C-AF67-291303C93628}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D236BB9-FBA6-2148-B7AC-72790E059311}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14520" yWindow="580" windowWidth="19080" windowHeight="18860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="424">
   <si>
     <t>Data Category</t>
   </si>
@@ -1288,10 +1288,16 @@
     <t>Pasture 8B</t>
   </si>
   <si>
-    <t>Nautral Revegetation Exclosure</t>
-  </si>
-  <si>
     <t>Playas</t>
+  </si>
+  <si>
+    <t>Natural Revegetation Exclosure</t>
+  </si>
+  <si>
+    <t>SEL Bajada</t>
+  </si>
+  <si>
+    <t>Systems Ecology Lab</t>
   </si>
 </sst>
 </file>
@@ -1455,6 +1461,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1473,7 +1480,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1755,10 +1761,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:O48"/>
+  <dimension ref="A2:O49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I48" sqref="I48:J48"/>
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I49" sqref="I49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1813,47 +1819,47 @@
       <c r="L7" s="12"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="19" t="s">
         <v>350</v>
       </c>
-      <c r="B8" s="18"/>
+      <c r="B8" s="19"/>
       <c r="C8" s="4"/>
       <c r="D8" s="12"/>
-      <c r="E8" s="18" t="s">
+      <c r="E8" s="19" t="s">
         <v>387</v>
       </c>
-      <c r="F8" s="18"/>
+      <c r="F8" s="19"/>
       <c r="H8" s="12"/>
-      <c r="I8" s="18" t="s">
+      <c r="I8" s="19" t="s">
         <v>386</v>
       </c>
-      <c r="J8" s="18"/>
+      <c r="J8" s="19"/>
       <c r="L8" s="12"/>
-      <c r="M8" s="19" t="s">
+      <c r="M8" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="N8" s="19"/>
+      <c r="N8" s="20"/>
     </row>
     <row r="9" spans="1:15" s="5" customFormat="1" ht="47" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="15" t="s">
         <v>407</v>
       </c>
-      <c r="B9" s="15"/>
+      <c r="B9" s="16"/>
       <c r="D9" s="13"/>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="15" t="s">
         <v>358</v>
       </c>
-      <c r="F9" s="15"/>
+      <c r="F9" s="16"/>
       <c r="H9" s="13"/>
-      <c r="I9" s="14" t="s">
+      <c r="I9" s="15" t="s">
         <v>358</v>
       </c>
-      <c r="J9" s="15"/>
+      <c r="J9" s="16"/>
       <c r="L9" s="13"/>
-      <c r="M9" s="16" t="s">
+      <c r="M9" s="17" t="s">
         <v>383</v>
       </c>
-      <c r="N9" s="17"/>
+      <c r="N9" s="18"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
@@ -2426,6 +2432,12 @@
       <c r="C29" s="6" t="s">
         <v>406</v>
       </c>
+      <c r="E29" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>387</v>
+      </c>
       <c r="I29" s="2" t="s">
         <v>357</v>
       </c>
@@ -2520,6 +2532,12 @@
       <c r="O33" s="6"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A34" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>350</v>
+      </c>
       <c r="C34" s="6"/>
       <c r="I34" s="2" t="s">
         <v>418</v>
@@ -2652,7 +2670,7 @@
     </row>
     <row r="47" spans="1:15" ht="15" x14ac:dyDescent="0.2">
       <c r="I47" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="J47" s="2" t="s">
         <v>386</v>
@@ -2661,9 +2679,17 @@
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.15">
       <c r="I48" s="2" t="s">
-        <v>421</v>
-      </c>
-      <c r="J48" s="20" t="s">
+        <v>420</v>
+      </c>
+      <c r="J48" s="14" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="49" spans="9:10" x14ac:dyDescent="0.15">
+      <c r="I49" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="J49" s="14" t="s">
         <v>386</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding some old project names
</commit_message>
<xml_diff>
--- a/standards/keyword_thesauri.xlsx
+++ b/standards/keyword_thesauri.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10810"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmaurer/GitHub/documentation/standards/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DataProducts/LTER_IM/documentation/standards/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D236BB9-FBA6-2148-B7AC-72790E059311}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06361600-E61D-FB44-B157-96326279FCB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14520" yWindow="580" windowWidth="19080" windowHeight="18860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,17 +16,25 @@
     <sheet name="Current_Thesauri" sheetId="2" r:id="rId1"/>
     <sheet name="Old_DEIMS_Thesauri" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="426">
   <si>
     <t>Data Category</t>
   </si>
@@ -1298,6 +1306,12 @@
   </si>
   <si>
     <t>Systems Ecology Lab</t>
+  </si>
+  <si>
+    <t>Mesquite phenology</t>
+  </si>
+  <si>
+    <t>Fluffgrass</t>
   </si>
 </sst>
 </file>
@@ -1763,8 +1777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:O49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I49" sqref="I49"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -2457,6 +2471,12 @@
       <c r="C30" s="6" t="s">
         <v>406</v>
       </c>
+      <c r="E30" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>387</v>
+      </c>
       <c r="I30" s="2" t="s">
         <v>372</v>
       </c>
@@ -2477,6 +2497,12 @@
       </c>
       <c r="C31" s="6" t="s">
         <v>406</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>387</v>
       </c>
       <c r="I31" s="2" t="s">
         <v>373</v>

</xml_diff>